<commit_message>
Schedule Management file is updated according to the cost estimation file.
</commit_message>
<xml_diff>
--- a/Schedule Management.xlsx
+++ b/Schedule Management.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538343\Documents\691\44691-Module1-Badami4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538306\Documents\Annie_Documents\691\44691-Module1-Badami4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512F4FEA-DCF2-4900-BA99-CD89FCA1E416}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89069AE4-BCF1-4BB4-8BBC-0C803D56BC5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -273,6 +273,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -282,11 +287,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1380,18 +1380,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20" x14ac:dyDescent="0.4">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -1410,12 +1410,12 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="15"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
@@ -1642,10 +1642,10 @@
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="13">
         <v>44162</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="14" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1854,7 +1854,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="7"/>

</xml_diff>